<commit_message>
1213 B win AI
</commit_message>
<xml_diff>
--- a/자가채점표(1조).xlsx
+++ b/자가채점표(1조).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="HCell" lastEdited="12.0" lowestEdited="12.0" rupBuild="0.893"/>
+  <x:fileVersion appName="HCell" lastEdited="12.0" lowestEdited="12.0" rupBuild="0.4204"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimmi\Desktop\GitHub\Multi2_Team1_2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimmi\Desktop\과제\Multi2_Team1_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="17724" windowHeight="6348" activeTab="1"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="17715" windowHeight="6330" activeTab="1"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="5인조" sheetId="1" r:id="rId4"/>
@@ -22,78 +22,78 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <x:si>
+    <x:t>1조</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이름</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이종석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>김유미</x:t>
+  </x:si>
+  <x:si>
+    <x:t>학번</x:t>
+  </x:si>
+  <x:si>
+    <x:t>홍주아</x:t>
+  </x:si>
+  <x:si>
+    <x:t>김유민</x:t>
+  </x:si>
+  <x:si>
+    <x:t>총합</x:t>
+  </x:si>
+  <x:si>
     <x:t>조원이 4인인 조는 이 페이지에 작성해주세요
 각 엑셀에는 참여한 학생의 참여율을 적어주세요. (잘 모를땐 25%로 공평하게)
 문제의 총 참여율은 100%가 되어야합니다. 각 해금문제는 10점씩, 게임AI는 20점 배점을 드립니다.</x:t>
   </x:si>
   <x:si>
+    <x:t>(조이름) 정신나간조</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3번문제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7번문제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4번문제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1번문제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>으야야야아아</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5번문제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>으랴아아아아</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2번문제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6번문제</x:t>
+  </x:si>
+  <x:si>
     <x:t>갸아아아아아</x:t>
   </x:si>
   <x:si>
-    <x:t>으랴아아아아</x:t>
-  </x:si>
-  <x:si>
-    <x:t>으야야야아아</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4번문제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3번문제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7번문제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2번문제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1번문제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5번문제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6번문제</x:t>
+    <x:t>8번문제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게임AI</x:t>
   </x:si>
   <x:si>
     <x:t>이야야야야야</x:t>
   </x:si>
   <x:si>
-    <x:t>8번문제</x:t>
-  </x:si>
-  <x:si>
     <x:t>냐아아아아아</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게임AI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>학번</x:t>
-  </x:si>
-  <x:si>
-    <x:t>김유미</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이름</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1조</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이종석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>총합</x:t>
-  </x:si>
-  <x:si>
-    <x:t>홍주아</x:t>
-  </x:si>
-  <x:si>
-    <x:t>김유민</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(조이름) 정신나간조</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -195,8 +195,406 @@
   <x:cellStyles count="1">
     <x:cellStyle name="표준" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:dxfs count="0"/>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:dxfs count="12">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:dxf hs:applyExtension="1">
+          <x:font hs:extension="1">
+            <x:color rgb="ff000000"/>
+            <hs:useFontSpace val="0"/>
+            <hs:size val="0"/>
+            <hs:ratio val="0"/>
+            <hs:spacing val="0"/>
+            <hs:offset val="0"/>
+          </x:font>
+          <x:fill>
+            <x:patternFill patternType="solid">
+              <x:fgColor rgb="ffd7dff4"/>
+              <x:bgColor rgb="ffd7dff4"/>
+            </x:patternFill>
+          </x:fill>
+          <x:border>
+            <x:left style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:left>
+            <x:right style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:right>
+            <x:top style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:top>
+            <x:bottom style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:bottom>
+            <x:vertical style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:vertical>
+            <x:horizontal style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:horizontal>
+          </x:border>
+        </x:dxf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:dxf>
+          <x:font>
+            <x:color rgb="ff000000"/>
+          </x:font>
+          <x:fill>
+            <x:patternFill patternType="solid">
+              <x:fgColor rgb="ffd7dff4"/>
+              <x:bgColor rgb="ffd7dff4"/>
+            </x:patternFill>
+          </x:fill>
+          <x:border>
+            <x:left style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:left>
+            <x:right style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:right>
+            <x:top style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:top>
+            <x:bottom style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:bottom>
+            <x:vertical style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:vertical>
+            <x:horizontal style="thin">
+              <x:color rgb="ffffffff"/>
+            </x:horizontal>
+          </x:border>
+        </x:dxf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:dxf/>
+    <x:dxf>
+      <x:fill>
+        <x:patternFill patternType="solid">
+          <x:fgColor rgb="ffaebfea"/>
+          <x:bgColor rgb="ffaebfea"/>
+        </x:patternFill>
+      </x:fill>
+    </x:dxf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:dxf hs:applyExtension="1">
+          <x:font hs:extension="1">
+            <x:color rgb="ffffffff"/>
+            <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
+            <hs:size val="0"/>
+            <hs:ratio val="0"/>
+            <hs:spacing val="0"/>
+            <hs:offset val="0"/>
+          </x:font>
+          <x:fill>
+            <x:patternFill patternType="solid">
+              <x:fgColor rgb="ff6182d6"/>
+              <x:bgColor rgb="ff6182d6"/>
+            </x:patternFill>
+          </x:fill>
+        </x:dxf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:dxf>
+          <x:font>
+            <x:color rgb="ffffffff"/>
+            <x:b val="1"/>
+          </x:font>
+          <x:fill>
+            <x:patternFill patternType="solid">
+              <x:fgColor rgb="ff6182d6"/>
+              <x:bgColor rgb="ff6182d6"/>
+            </x:patternFill>
+          </x:fill>
+        </x:dxf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:dxf hs:applyExtension="1">
+          <x:font hs:extension="1">
+            <x:color rgb="ffffffff"/>
+            <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
+            <hs:size val="0"/>
+            <hs:ratio val="0"/>
+            <hs:spacing val="0"/>
+            <hs:offset val="0"/>
+          </x:font>
+          <x:fill>
+            <x:patternFill patternType="solid">
+              <x:fgColor rgb="ff6182d6"/>
+              <x:bgColor rgb="ff6182d6"/>
+            </x:patternFill>
+          </x:fill>
+          <x:border>
+            <x:top style="thick">
+              <x:color rgb="ffffffff"/>
+            </x:top>
+          </x:border>
+        </x:dxf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:dxf>
+          <x:font>
+            <x:color rgb="ffffffff"/>
+            <x:b val="1"/>
+          </x:font>
+          <x:fill>
+            <x:patternFill patternType="solid">
+              <x:fgColor rgb="ff6182d6"/>
+              <x:bgColor rgb="ff6182d6"/>
+            </x:patternFill>
+          </x:fill>
+          <x:border>
+            <x:top style="thick">
+              <x:color rgb="ffffffff"/>
+            </x:top>
+          </x:border>
+        </x:dxf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:dxf hs:applyExtension="1">
+          <x:font hs:extension="1">
+            <x:color rgb="ffffffff"/>
+            <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
+            <hs:size val="0"/>
+            <hs:ratio val="0"/>
+            <hs:spacing val="0"/>
+            <hs:offset val="0"/>
+          </x:font>
+          <x:fill>
+            <x:patternFill patternType="solid">
+              <x:fgColor rgb="ff6182d6"/>
+              <x:bgColor rgb="ff6182d6"/>
+            </x:patternFill>
+          </x:fill>
+          <x:border>
+            <x:bottom style="thick">
+              <x:color rgb="ffffffff"/>
+            </x:bottom>
+          </x:border>
+        </x:dxf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:dxf>
+          <x:font>
+            <x:color rgb="ffffffff"/>
+            <x:b val="1"/>
+          </x:font>
+          <x:fill>
+            <x:patternFill patternType="solid">
+              <x:fgColor rgb="ff6182d6"/>
+              <x:bgColor rgb="ff6182d6"/>
+            </x:patternFill>
+          </x:fill>
+          <x:border>
+            <x:bottom style="thick">
+              <x:color rgb="ffffffff"/>
+            </x:bottom>
+          </x:border>
+        </x:dxf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:dxf hs:applyExtension="1">
+          <x:font hs:extension="1">
+            <x:color rgb="ff000000"/>
+            <hs:useFontSpace val="0"/>
+            <hs:size val="0"/>
+            <hs:ratio val="0"/>
+            <hs:spacing val="0"/>
+            <hs:offset val="0"/>
+          </x:font>
+          <x:border>
+            <x:left>
+              <x:color auto="1"/>
+            </x:left>
+            <x:right>
+              <x:color auto="1"/>
+            </x:right>
+            <x:top style="medium">
+              <x:color rgb="ff6182d6"/>
+            </x:top>
+            <x:bottom style="medium">
+              <x:color rgb="ff6182d6"/>
+            </x:bottom>
+            <x:vertical>
+              <x:color auto="1"/>
+            </x:vertical>
+            <x:horizontal>
+              <x:color auto="1"/>
+            </x:horizontal>
+          </x:border>
+        </x:dxf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:dxf>
+          <x:font>
+            <x:color rgb="ff000000"/>
+          </x:font>
+          <x:border>
+            <x:left>
+              <x:color auto="1"/>
+            </x:left>
+            <x:right>
+              <x:color auto="1"/>
+            </x:right>
+            <x:top style="medium">
+              <x:color rgb="ff6182d6"/>
+            </x:top>
+            <x:bottom style="medium">
+              <x:color rgb="ff6182d6"/>
+            </x:bottom>
+            <x:vertical>
+              <x:color auto="1"/>
+            </x:vertical>
+            <x:horizontal>
+              <x:color auto="1"/>
+            </x:horizontal>
+          </x:border>
+        </x:dxf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:dxf>
+      <x:fill>
+        <x:patternFill patternType="solid">
+          <x:fgColor rgb="ff94a5df"/>
+          <x:bgColor rgb="ff94a5df"/>
+        </x:patternFill>
+      </x:fill>
+      <x:border>
+        <x:top style="thin">
+          <x:color rgb="ff6182d6"/>
+        </x:top>
+        <x:bottom style="thin">
+          <x:color rgb="ff6182d6"/>
+        </x:bottom>
+      </x:border>
+    </x:dxf>
+    <x:dxf>
+      <x:fill>
+        <x:patternFill patternType="solid">
+          <x:fgColor rgb="ff6182d6"/>
+          <x:bgColor rgb="ff6182d6"/>
+        </x:patternFill>
+      </x:fill>
+    </x:dxf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:dxf hs:applyExtension="1">
+          <x:font hs:extension="1">
+            <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
+            <hs:size val="0"/>
+            <hs:ratio val="0"/>
+            <hs:spacing val="0"/>
+            <hs:offset val="0"/>
+          </x:font>
+        </x:dxf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:dxf>
+          <x:font>
+            <x:b val="1"/>
+          </x:font>
+        </x:dxf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:dxf hs:applyExtension="1">
+          <x:font hs:extension="1">
+            <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
+            <hs:size val="0"/>
+            <hs:ratio val="0"/>
+            <hs:spacing val="0"/>
+            <hs:offset val="0"/>
+          </x:font>
+          <x:border>
+            <x:top style="thin">
+              <x:color rgb="ff6182d6"/>
+            </x:top>
+          </x:border>
+        </x:dxf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:dxf>
+          <x:font>
+            <x:b val="1"/>
+          </x:font>
+          <x:border>
+            <x:top style="thin">
+              <x:color rgb="ff6182d6"/>
+            </x:top>
+          </x:border>
+        </x:dxf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:dxf hs:applyExtension="1">
+          <x:font hs:extension="1">
+            <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
+            <hs:size val="0"/>
+            <hs:ratio val="0"/>
+            <hs:spacing val="0"/>
+            <hs:offset val="0"/>
+          </x:font>
+          <x:border>
+            <x:bottom style="medium">
+              <x:color rgb="ff6182d6"/>
+            </x:bottom>
+          </x:border>
+        </x:dxf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:dxf>
+          <x:font>
+            <x:b val="1"/>
+          </x:font>
+          <x:border>
+            <x:bottom style="medium">
+              <x:color rgb="ff6182d6"/>
+            </x:bottom>
+          </x:border>
+        </x:dxf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </x:dxfs>
+  <x:tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <x:tableStyle name="Normal Style 1 - Accent 1" pivot="0" table="1" count="9">
+      <x:tableStyleElement type="wholeTable" size="1" dxfId="0"/>
+      <x:tableStyleElement type="headerRow" size="1" dxfId="5"/>
+      <x:tableStyleElement type="totalRow" size="1" dxfId="4"/>
+      <x:tableStyleElement type="firstColumn" size="1" dxfId="3"/>
+      <x:tableStyleElement type="lastColumn" size="1" dxfId="3"/>
+      <x:tableStyleElement type="firstRowStripe" size="1" dxfId="2"/>
+      <x:tableStyleElement type="secondRowStripe" size="1" dxfId="1"/>
+      <x:tableStyleElement type="firstColumnStripe" size="1" dxfId="2"/>
+      <x:tableStyleElement type="secondColumnStripe" size="1" dxfId="1"/>
+    </x:tableStyle>
+    <x:tableStyle name="Light Style 1 - Accent 1" pivot="1" table="0" count="8">
+      <x:tableStyleElement type="wholeTable" size="1" dxfId="6"/>
+      <x:tableStyleElement type="headerRow" size="1" dxfId="11"/>
+      <x:tableStyleElement type="totalRow" size="1" dxfId="10"/>
+      <x:tableStyleElement type="firstColumn" size="1" dxfId="9"/>
+      <x:tableStyleElement type="lastColumn" size="1" dxfId="9"/>
+      <x:tableStyleElement type="firstRowStripe" size="1" dxfId="7"/>
+      <x:tableStyleElement type="secondRowStripe" size="1" dxfId="1"/>
+      <x:tableStyleElement type="firstColumnStripe" size="1" dxfId="8"/>
+    </x:tableStyle>
+  </x:tableStyles>
 </x:styleSheet>
 </file>
 
@@ -493,26 +891,26 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="A1:L14"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <x:sheetView topLeftCell="A1" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <x:selection activeCell="A7" activeCellId="0" sqref="A7:A7"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="17"/>
+  <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="16.39999999999999857891"/>
   <x:cols>
     <x:col min="2" max="2" width="18.83203125" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" t="s">
-        <x:v>18</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B1" t="s">
-        <x:v>23</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
       <x:c r="A3" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B3" s="2"/>
       <x:c r="C3" s="2"/>
@@ -562,40 +960,40 @@
     </x:row>
     <x:row r="8" spans="1:12">
       <x:c r="A8" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B8" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C8" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D8" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E8" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F8" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G8" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="B8" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C8" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D8" t="s">
+      <x:c r="H8" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="I8" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="J8" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K8" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L8" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E8" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="F8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="G8" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="H8" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="I8" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="J8" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="K8" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="L8" t="s">
-        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:12">
@@ -603,7 +1001,7 @@
         <x:v>1212121</x:v>
       </x:c>
       <x:c r="B9" t="s">
-        <x:v>3</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C9">
         <x:v>20</x:v>
@@ -642,7 +1040,7 @@
         <x:v>1212122</x:v>
       </x:c>
       <x:c r="B10" t="s">
-        <x:v>11</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C10">
         <x:v>20</x:v>
@@ -681,7 +1079,7 @@
         <x:v>1212123</x:v>
       </x:c>
       <x:c r="B11" t="s">
-        <x:v>2</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C11">
         <x:v>20</x:v>
@@ -720,7 +1118,7 @@
         <x:v>1212124</x:v>
       </x:c>
       <x:c r="B12" t="s">
-        <x:v>1</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C12">
         <x:v>20</x:v>
@@ -759,7 +1157,7 @@
         <x:v>1212125</x:v>
       </x:c>
       <x:c r="B13" t="s">
-        <x:v>13</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C13">
         <x:v>20</x:v>
@@ -835,7 +1233,7 @@
   <x:mergeCells count="1">
     <x:mergeCell ref="A3:J6"/>
   </x:mergeCells>
-  <x:pageMargins left="0.69999998807907104492" right="0.69999998807907104492" top="0.75" bottom="0.75" header="0.30000001192092895508" footer="0.30000001192092895508"/>
+  <x:pageMargins left="0.69986110925674438477" right="0.69986110925674438477" top="0.75" bottom="0.75" header="0.30000001192092895508" footer="0.30000001192092895508"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -845,26 +1243,27 @@
   <x:sheetPr codeName="Sheet2"/>
   <x:dimension ref="A1:L13"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="K11" activeCellId="0" sqref="K11:K11"/>
+    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <x:selection activeCell="N8" activeCellId="0" sqref="N8:N8"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="16.39999999999999857891"/>
   <x:cols>
     <x:col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <x:col min="11" max="11" width="8.796875" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" t="s">
-        <x:v>18</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B1" t="s">
-        <x:v>18</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
       <x:c r="A3" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B3" s="2"/>
       <x:c r="C3" s="2"/>
@@ -914,40 +1313,40 @@
     </x:row>
     <x:row r="8" spans="1:12">
       <x:c r="A8" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B8" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C8" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D8" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E8" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F8" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G8" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="B8" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C8" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D8" t="s">
+      <x:c r="H8" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="I8" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="J8" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="K8" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L8" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E8" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="F8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="G8" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="H8" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="I8" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="J8" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="K8" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="L8" t="s">
-        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:12">
@@ -955,7 +1354,7 @@
         <x:v>20251389</x:v>
       </x:c>
       <x:c r="B9" t="s">
-        <x:v>16</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C9">
         <x:v>0</x:v>
@@ -982,11 +1381,11 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="K9">
-        <x:v>0</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="L9">
         <x:f>(SUM(C9:J9)*10+(K9*20))/25</x:f>
-        <x:v>80</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:12">
@@ -994,7 +1393,7 @@
         <x:v>20251398</x:v>
       </x:c>
       <x:c r="B10" t="s">
-        <x:v>21</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C10">
         <x:v>0</x:v>
@@ -1021,11 +1420,11 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K10">
-        <x:v>0</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="L10">
         <x:f t="shared" ref="L10:L12" si="0">(SUM(C10:J10)*10+(K10*20))/25</x:f>
-        <x:v>80</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:12">
@@ -1033,7 +1432,7 @@
         <x:v>20251402</x:v>
       </x:c>
       <x:c r="B11" t="s">
-        <x:v>22</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C11">
         <x:v>100</x:v>
@@ -1060,11 +1459,11 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K11">
-        <x:v>0</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="L11">
         <x:f t="shared" si="0"/>
-        <x:v>80</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:12">
@@ -1072,7 +1471,7 @@
         <x:v>20251413</x:v>
       </x:c>
       <x:c r="B12" t="s">
-        <x:v>19</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="C12">
         <x:v>0</x:v>
@@ -1099,11 +1498,11 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K12">
-        <x:v>0</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="L12">
         <x:f t="shared" si="0"/>
-        <x:v>80</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="3:11">
@@ -1141,14 +1540,14 @@
       </x:c>
       <x:c r="K13">
         <x:f t="shared" si="1"/>
-        <x:v>0</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="1">
     <x:mergeCell ref="A3:J6"/>
   </x:mergeCells>
-  <x:pageMargins left="0.69999998807907104492" right="0.69999998807907104492" top="0.75" bottom="0.75" header="0.30000001192092895508" footer="0.30000001192092895508"/>
+  <x:pageMargins left="0.69986110925674438477" right="0.69986110925674438477" top="0.75" bottom="0.75" header="0.30000001192092895508" footer="0.30000001192092895508"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>